<commit_message>
Gráficos en Excel, conexión entre diseños columnas y círculos
</commit_message>
<xml_diff>
--- a/6. Funciones-en-Excel-MIN-MO-M-XIMO.PROMEDIO-y-CONTAR.xlsx.xlsx
+++ b/6. Funciones-en-Excel-MIN-MO-M-XIMO.PROMEDIO-y-CONTAR.xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PAUL\Downloads\Materiales-Para-Descargar\Curso_excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AB5798-D149-462B-BB9E-8C96F458D4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C55CD9F6-8D8C-478B-9A90-20BE7E4D545E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="11625" xr2:uid="{387765B8-A6D8-4B9F-8E14-1C810584CD88}"/>
   </bookViews>
@@ -274,6 +274,4196 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mantenimiento</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Publicidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Personal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Papeleria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Eventos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$9:$G$9</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2300</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Diseños</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$10:$G$10</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Agencias</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$11:$G$11</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000006-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Redes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$12:$G$12</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000007-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Contabilidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:solidFill>
+                <a:sysClr val="window" lastClr="FFFFFF"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="25000"/>
+                    <a:lumOff val="75000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="1"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <a:prstGeom prst="wedgeRectCallout">
+                    <a:avLst/>
+                  </a:prstGeom>
+                  <a:noFill/>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                </c15:spPr>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>43101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43132</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43160</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$B$13:$G$13</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000008-F81A-41FB-AD35-11904B5C15BD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="0"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="es-ES"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="es-PE" sz="2800"/>
+              <a:t>Parque</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-PE" sz="2800" baseline="0"/>
+              <a:t> Infantil</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-PE" sz="2800"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2800" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Mantenimiento</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>700</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-21CB-4C7B-A182-736EE111D413}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Publicidad</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$6:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>6000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-21CB-4C7B-A182-736EE111D413}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Personal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent6">
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$7:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-21CB-4C7B-A182-736EE111D413}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Presupuesto1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Papeleria</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+            </a:ln>
+            <a:effectLst>
+              <a:glow rad="63500">
+                <a:schemeClr val="accent4">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="25000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>mmm\-yyyy</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>43191</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43221</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43252</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Presupuesto1!$E$8:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>[$$-409]#,##0.00</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-21CB-4C7B-A182-736EE111D413}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="315"/>
+        <c:overlap val="-40"/>
+        <c:axId val="724943807"/>
+        <c:axId val="724944223"/>
+      </c:barChart>
+      <c:dateAx>
+        <c:axId val="724943807"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="mmm\-yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724944223"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="months"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="724944223"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Gastos</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-PE" baseline="0"/>
+                  <a:t> e Inversión</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="es-PE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="[$$-409]#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-PE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="724943807"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-PE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-PE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="213">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="4"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="65000"/>
+                <a:lumOff val="35000"/>
+                <a:alpha val="25000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4042,6 +8232,42 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>92867</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>150018</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>319086</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>33338</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Gráfico 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4D06CDA-F723-474D-AC49-633DE7B16A05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4049,16 +8275,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>540543</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>102393</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>35717</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>130968</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>540543</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>130968</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>35717</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>159543</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4078,6 +8304,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
           <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId1" r:lo="rId2" r:qs="rId3" r:cs="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>500062</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26192</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>502443</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>109536</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{210BDE39-801B-4691-BA16-C06ABDD5DA05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4386,7 +8648,7 @@
   <dimension ref="A2:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4819,7 +9081,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>